<commit_message>
copied over local logsheets
</commit_message>
<xml_diff>
--- a/Course_Requirements/Activity Logs&Task Summaries/Jesse/Week_1_Logs.xlsx
+++ b/Course_Requirements/Activity Logs&Task Summaries/Jesse/Week_1_Logs.xlsx
@@ -1,19 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Documents\GitHub\CSC3600-ICT-Professional-Project\Course_Requirements\Activity Logs&amp;Task Summaries\Jesse\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9364CB6-96E2-4CF7-A453-4CB75F5A4B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="1480" windowWidth="25600" windowHeight="17460" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACTIVITY LOG SHEET " sheetId="1" r:id="rId1"/>
-    <sheet name="ACTIVITY LOG SHEET (sample)" sheetId="2" r:id="rId2"/>
-    <sheet name="TASK SUMMARY SHEET" sheetId="3" r:id="rId3"/>
-    <sheet name="ACTIVITY LOG SUMMARY SHEET" sheetId="4" r:id="rId4"/>
+    <sheet name="TASK SUMMARY SHEET" sheetId="3" r:id="rId2"/>
+    <sheet name="ACTIVITY LOG SUMMARY SHEET" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t xml:space="preserve">ACTIVITY LOG SHEET </t>
   </si>
@@ -67,45 +78,6 @@
   </si>
   <si>
     <t>Note:</t>
-  </si>
-  <si>
-    <t>Group meeting</t>
-  </si>
-  <si>
-    <t>Project management</t>
-  </si>
-  <si>
-    <t>GUI development</t>
-  </si>
-  <si>
-    <t>Meeting with supervisor</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Database connection</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 13:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 15:00:00</t>
-  </si>
-  <si>
-    <t>John Doe</t>
   </si>
   <si>
     <t>Task Summary Sheet</t>
@@ -191,23 +163,53 @@
     <t>• This sheet should be filled out in individual, weekly basis.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>• This sheet should be filled out in individual, whole-project basis. The data entered should be calculated based on weekly "Task Summary Sheet"</t>
   </si>
   <si>
     <t>• The overall laber cost of the project should be accumunated based on all members' "Activity Summary Sheet"s.</t>
+  </si>
+  <si>
+    <t>Jesse Hare</t>
+  </si>
+  <si>
+    <t>Group Meeting</t>
+  </si>
+  <si>
+    <t>Project Planning</t>
+  </si>
+  <si>
+    <t>Develop WBS</t>
+  </si>
+  <si>
+    <t>Meeting with Client</t>
+  </si>
+  <si>
+    <t>Req Analysis/elicitation</t>
+  </si>
+  <si>
+    <t>Proj Design</t>
+  </si>
+  <si>
+    <t>Develop WBS and project schedule</t>
+  </si>
+  <si>
+    <t>Conference with client to gather requirements, refine and model user tasks</t>
+  </si>
+  <si>
+    <t>Allocate team members, assign sprint master, setup per-team sprints</t>
+  </si>
+  <si>
+    <t>Proj Design Specifics</t>
+  </si>
+  <si>
+    <t>Design screen layours, choose framework, identify methods, classes and libraries required for core functionality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,12 +222,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -264,15 +268,18 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
@@ -283,6 +290,7 @@
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -296,6 +304,18 @@
     </font>
     <font>
       <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -739,7 +759,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -762,86 +782,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -926,6 +883,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -960,6 +959,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -980,7 +987,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Text 1"/>
+        <xdr:cNvPr id="2" name="Text 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1001,7 +1014,7 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
@@ -1359,46 +1372,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" thickTop="1" thickBot="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" ht="17" thickTop="1" thickBot="1">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="27" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-    </row>
-    <row r="3" spans="1:8" ht="32" thickTop="1" thickBot="1">
-      <c r="A3" s="8" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1418,145 +1431,145 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" thickTop="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+    <row r="4" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
       <c r="G5" s="5"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
       <c r="G8" s="5"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
       <c r="G9" s="5"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="54"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="G10" s="5"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="54"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="54"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="5"/>
       <c r="F14" s="6"/>
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
       <c r="G15" s="5"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+    <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="59"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="7"/>
       <c r="F16" s="2"/>
       <c r="G16" s="7"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
       <c r="G17" s="2">
         <f>SUM(G4:G16)</f>
         <v>0</v>
@@ -1566,39 +1579,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16" thickTop="1"/>
-    <row r="19" spans="1:8">
+    <row r="18" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
@@ -1606,6 +1614,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
@@ -1623,318 +1636,225 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" thickTop="1" thickBot="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="16">
+        <v>1</v>
+      </c>
+      <c r="F1" s="20"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="26">
+        <v>4</v>
+      </c>
+      <c r="D3" s="26">
+        <v>4</v>
+      </c>
+      <c r="E3" s="26">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" ht="17" thickTop="1" thickBot="1">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="26">
+        <v>2</v>
+      </c>
+      <c r="D4" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="E4" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="26">
+        <v>5</v>
+      </c>
+      <c r="D5" s="26">
+        <v>4</v>
+      </c>
+      <c r="E5" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="26">
+        <v>3</v>
+      </c>
+      <c r="D6" s="26">
+        <v>4</v>
+      </c>
+      <c r="E6" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="27"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+    </row>
+    <row r="8" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="27"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="27"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+    </row>
+    <row r="11" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="27"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+    </row>
+    <row r="12" spans="1:8" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="27"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" s="17" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+    </row>
+    <row r="14" spans="1:8" s="17" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14"/>
+      <c r="C14" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="32">
+        <f>SUM(D3:D13)</f>
+        <v>13</v>
+      </c>
+      <c r="E14" s="33"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="14">
-        <v>7</v>
-      </c>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" ht="32" thickTop="1" thickBot="1">
-      <c r="A3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" thickTop="1">
-      <c r="A4" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="28">
-        <v>42604</v>
-      </c>
-      <c r="E4" s="30">
-        <v>0.375</v>
-      </c>
-      <c r="F4" s="31">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="29">
-        <v>42604</v>
-      </c>
-      <c r="E5" s="30">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="F5" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="29">
-        <v>42604</v>
-      </c>
-      <c r="E6" s="30">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F6" s="31">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="29">
-        <v>42605</v>
-      </c>
-      <c r="E7" s="30">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="29">
-        <v>42605</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="29">
-        <v>42605</v>
-      </c>
-      <c r="E9" s="30" t="s">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="31" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="2">
-        <f>SUM(G4:G16)</f>
-        <v>2</v>
-      </c>
-      <c r="H17" s="2">
-        <f>SUM(H4:H16)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="16" thickTop="1"/>
-    <row r="25" spans="1:11">
-      <c r="K25" t="s">
-        <v>49</v>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1944,288 +1864,124 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="39.5" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="22" thickBot="1">
-      <c r="A1" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="41"/>
-      <c r="H1" s="42"/>
-    </row>
-    <row r="2" spans="1:8" ht="41" thickBot="1">
-      <c r="A2" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-    </row>
-    <row r="4" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A4" s="48"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-    </row>
-    <row r="5" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A5" s="48"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-    </row>
-    <row r="6" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A6" s="48"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-    </row>
-    <row r="7" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A7" s="48"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-    </row>
-    <row r="8" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A8" s="48"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-    </row>
-    <row r="9" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A9" s="48"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-    </row>
-    <row r="10" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A10" s="48"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-    </row>
-    <row r="11" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A11" s="48"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-    </row>
-    <row r="12" spans="1:8" s="38" customFormat="1" ht="21">
-      <c r="A12" s="48"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-    </row>
-    <row r="13" spans="1:8" s="38" customFormat="1" ht="22" thickBot="1">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-    </row>
-    <row r="14" spans="1:8" s="38" customFormat="1" ht="22" thickBot="1">
-      <c r="A14" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14"/>
-      <c r="C14" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="53">
-        <f>SUM(D3:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="54"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22" thickBot="1">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.4">
+      <c r="A4" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="39">
+        <v>1</v>
+      </c>
+      <c r="C4" s="40">
+        <v>0</v>
+      </c>
+      <c r="E4" s="41"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.4">
+      <c r="A5" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="39">
+        <v>4</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="E5" s="41"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.4">
+      <c r="A6" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="55"/>
-    </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1"/>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="57" t="s">
+      <c r="B6" s="39">
+        <v>2</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="E6" s="41"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.4">
+      <c r="A7" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="58" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="61"/>
-      <c r="E4" s="62"/>
-    </row>
-    <row r="5" spans="1:5" ht="28">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="61"/>
-      <c r="E5" s="62"/>
-    </row>
-    <row r="6" spans="1:5" ht="28">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="61"/>
-      <c r="E6" s="62"/>
-    </row>
-    <row r="7" spans="1:5" ht="28">
-      <c r="A7" s="59"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="61"/>
-      <c r="E7" s="62"/>
-    </row>
-    <row r="8" spans="1:5" ht="29" thickBot="1">
-      <c r="A8" s="59"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="61"/>
-      <c r="E8" s="62"/>
-    </row>
-    <row r="9" spans="1:5" ht="29" thickBot="1">
-      <c r="A9" s="59"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="63" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="62"/>
-    </row>
-    <row r="10" spans="1:5" ht="29" thickBot="1">
-      <c r="A10" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="65">
+      <c r="B7" s="39">
+        <v>1</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="E7" s="41"/>
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="40"/>
+      <c r="E8" s="41"/>
+    </row>
+    <row r="9" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="38"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="41"/>
+    </row>
+    <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="44">
         <f>SUM(B4:B9)</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="66">
+        <v>8</v>
+      </c>
+      <c r="C10" s="45">
         <f>SUM(C4:C9)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="53">
+      <c r="D10" s="32">
         <f>B10+C10</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="62"/>
-    </row>
-    <row r="12" spans="1:5" ht="23">
-      <c r="A12" s="67"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-    </row>
-    <row r="13" spans="1:5" s="67" customFormat="1" ht="23"/>
-    <row r="14" spans="1:5" s="67" customFormat="1" ht="23">
+        <v>8</v>
+      </c>
+      <c r="E10" s="41"/>
+    </row>
+    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="46"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2234,158 +1990,158 @@
       <c r="D14"/>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="15" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="16" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="17" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="18" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="19" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="20" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" s="67" customFormat="1" ht="23"/>
-    <row r="22" spans="1:5" s="67" customFormat="1" ht="23"/>
-    <row r="23" spans="1:5" s="67" customFormat="1" ht="23"/>
-    <row r="24" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="21" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="25" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="26" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="27" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="28" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="29" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="30" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="31" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:5" s="67" customFormat="1" ht="23">
+    <row r="32" spans="1:5" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" s="67" customFormat="1" ht="23">
+    <row r="33" spans="1:4" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" s="67" customFormat="1" ht="23">
+    <row r="34" spans="1:4" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" s="67" customFormat="1" ht="23">
+    <row r="35" spans="1:4" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" s="67" customFormat="1" ht="23">
+    <row r="36" spans="1:4" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" s="67" customFormat="1" ht="23">
+    <row r="37" spans="1:4" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" s="67" customFormat="1" ht="23">
+    <row r="38" spans="1:4" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" s="67" customFormat="1" ht="23">
+    <row r="39" spans="1:4" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" s="67" customFormat="1" ht="23">
+    <row r="40" spans="1:4" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>

</xml_diff>